<commit_message>
Class Directory added, amongst other things
</commit_message>
<xml_diff>
--- a/Semester_3/Biology_Practicals/Analysis/Taste/Book2.xlsx
+++ b/Semester_3/Biology_Practicals/Analysis/Taste/Book2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Biplob</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t>Athira John</t>
+  </si>
+  <si>
+    <t>Athira Niar</t>
   </si>
 </sst>
 </file>
@@ -432,15 +438,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -471,7 +478,7 @@
         <v>27</v>
       </c>
       <c r="D2">
-        <f>AVERAGE(B2:C2)</f>
+        <f t="shared" ref="D2:D18" si="0">AVERAGE(B2:C2)</f>
         <v>23</v>
       </c>
       <c r="E2" t="s">
@@ -489,7 +496,7 @@
         <v>37</v>
       </c>
       <c r="D3">
-        <f>AVERAGE(B3:C3)</f>
+        <f t="shared" si="0"/>
         <v>29.5</v>
       </c>
       <c r="E3" t="s">
@@ -510,7 +517,7 @@
         <v>27</v>
       </c>
       <c r="D4">
-        <f>AVERAGE(B4:C4)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="E4" t="s">
@@ -528,7 +535,7 @@
         <v>18</v>
       </c>
       <c r="D5">
-        <f>AVERAGE(B5:C5)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E5" t="s">
@@ -546,7 +553,7 @@
         <v>44</v>
       </c>
       <c r="D6">
-        <f>AVERAGE(B6:C6)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="E6" t="s">
@@ -564,7 +571,7 @@
         <v>31</v>
       </c>
       <c r="D7">
-        <f>AVERAGE(B7:C7)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="E7" t="s">
@@ -579,7 +586,7 @@
         <v>35</v>
       </c>
       <c r="D8">
-        <f>AVERAGE(B8:C8)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
@@ -594,7 +601,7 @@
         <v>54</v>
       </c>
       <c r="D9">
-        <f>AVERAGE(B9:C9)</f>
+        <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
       <c r="E9" t="s">
@@ -612,7 +619,7 @@
         <v>44</v>
       </c>
       <c r="D10">
-        <f>AVERAGE(B10:C10)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="E10" t="s">
@@ -630,7 +637,7 @@
         <v>41</v>
       </c>
       <c r="D11">
-        <f>AVERAGE(B11:C11)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="E11" t="s">
@@ -648,7 +655,7 @@
         <v>32</v>
       </c>
       <c r="D12">
-        <f>AVERAGE(B12:C12)</f>
+        <f t="shared" si="0"/>
         <v>46.5</v>
       </c>
       <c r="E12" t="s">
@@ -672,7 +679,7 @@
         <v>54</v>
       </c>
       <c r="D13">
-        <f>AVERAGE(B13:C13)</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="E13" t="s">
@@ -690,8 +697,11 @@
         <v>65</v>
       </c>
       <c r="D14">
-        <f>AVERAGE(B14:C14)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
       </c>
       <c r="F14">
         <v>37</v>
@@ -708,7 +718,7 @@
         <v>112</v>
       </c>
       <c r="D15">
-        <f>AVERAGE(B15:C15)</f>
+        <f t="shared" si="0"/>
         <v>108.5</v>
       </c>
       <c r="E15" t="s">
@@ -723,7 +733,7 @@
         <v>113</v>
       </c>
       <c r="D16">
-        <f>AVERAGE(B16:C16)</f>
+        <f t="shared" si="0"/>
         <v>113</v>
       </c>
       <c r="E16" t="s">
@@ -731,6 +741,42 @@
       </c>
       <c r="G16" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completing the physics record plus bio amongst other things
</commit_message>
<xml_diff>
--- a/Semester_3/Biology_Practicals/Analysis/Taste/Book2.xlsx
+++ b/Semester_3/Biology_Practicals/Analysis/Taste/Book2.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A. S. Aurora\Documents\IISER_repo\Semester_3\Biology_Practicals\Analysis\Taste\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="375" windowWidth="17955" windowHeight="8730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Biplob</t>
   </si>
@@ -100,6 +105,18 @@
   </si>
   <si>
     <t>Athira Niar</t>
+  </si>
+  <si>
+    <t>Tasters</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Mean Sample</t>
+  </si>
+  <si>
+    <t>Variance</t>
   </si>
 </sst>
 </file>
@@ -146,6 +163,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -194,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,7 +249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,19 +458,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -466,8 +487,17 @@
       <c r="G1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -478,14 +508,29 @@
         <v>27</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D18" si="0">AVERAGE(B2:C2)</f>
+        <f>AVERAGE(B2:C2)</f>
         <v>23</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>_xlfn.VAR.S(D2:D8)</f>
+        <v>861.66666666666663</v>
+      </c>
+      <c r="J2">
+        <f>_xlfn.STDEV.S(D2:D8)</f>
+        <v>29.354159273715652</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(D2:D8)</f>
+        <v>43.5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -496,7 +541,7 @@
         <v>37</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B3:C3)</f>
         <v>29.5</v>
       </c>
       <c r="E3" t="s">
@@ -505,8 +550,23 @@
       <c r="G3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f>_xlfn.VAR.S(D9:D18)</f>
+        <v>590.22500000000014</v>
+      </c>
+      <c r="J3">
+        <f>_xlfn.STDEV.S(D9:D18)</f>
+        <v>24.294546713202948</v>
+      </c>
+      <c r="K3">
+        <f>AVERAGE(D9:D18)</f>
+        <v>47.85</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -517,14 +577,14 @@
         <v>27</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B4:C4)</f>
         <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -535,128 +595,138 @@
         <v>18</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B5:C5)</f>
         <v>33</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <f>AVERAGE(B6:C6)</f>
+        <v>37.5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGE(D2:D18)</f>
+        <v>46.058823529411768</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>41</v>
+      </c>
+      <c r="D7">
+        <f>AVERAGE(B7:C7)</f>
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>105</v>
+      </c>
+      <c r="C8">
+        <v>112</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(B8:C8)</f>
+        <v>108.5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>65</v>
+      </c>
+      <c r="D9">
+        <f>AVERAGE(B9:C9)</f>
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>113</v>
+      </c>
+      <c r="D10">
+        <f>AVERAGE(B10:C10)</f>
+        <v>113</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
+      <c r="B11">
         <v>22</v>
       </c>
-      <c r="C6">
+      <c r="C11">
         <v>44</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
+      <c r="D11">
+        <f>AVERAGE(B11:C11)</f>
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B12">
         <v>37</v>
       </c>
-      <c r="C7">
+      <c r="C12">
         <v>31</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
+      <c r="D12">
+        <f>AVERAGE(B12:C12)</f>
         <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>35</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>54</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>40</v>
-      </c>
-      <c r="C10">
-        <v>44</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>45</v>
-      </c>
-      <c r="C11">
-        <v>41</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>61</v>
-      </c>
-      <c r="C12">
-        <v>32</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>46.5</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -668,76 +738,79 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B13">
+        <v>40</v>
+      </c>
+      <c r="C13">
         <v>44</v>
       </c>
-      <c r="C13">
-        <v>54</v>
-      </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <f>AVERAGE(B13:C13)</f>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C14">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>57</v>
+        <f>AVERAGE(B14:C14)</f>
+        <v>46.5</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F14">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B15">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="C15">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>108.5</v>
+        <f>AVERAGE(B15:C15)</f>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>113</v>
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>38</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>113</v>
+        <f>AVERAGE(B16:C16)</f>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G16" t="s">
         <v>20</v>
@@ -745,17 +818,17 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C17">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <f>AVERAGE(B17:C17)</f>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -763,25 +836,19 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B18">
-        <v>31</v>
-      </c>
-      <c r="C18">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
+        <f>AVERAGE(B18:C18)</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J16">
-    <sortCondition ref="D2:D16"/>
+  <sortState ref="A2:E18">
+    <sortCondition ref="E2:E18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>